<commit_message>
almost ready to go
</commit_message>
<xml_diff>
--- a/experimental-scripts/psychopy/reading-experiment/reading-psychopy.xlsx
+++ b/experimental-scripts/psychopy/reading-experiment/reading-psychopy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ugentbe-my.sharepoint.com/personal/esperanza_badaya_ugent_be/Documents/Misc - Eye-tracking support/ugent-eyetracking/experimental-scripts/psychopy/reading-experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{F21EB3DC-0B57-4C59-B706-0F068D505D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5E44439-7EBD-47FC-AC3A-C684AD05F80E}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{F21EB3DC-0B57-4C59-B706-0F068D505D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CA1A450-7ABC-4AB4-A147-A91B028BCDD0}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{15E974C4-408E-4C2D-B569-14AE213A2C18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{15E974C4-408E-4C2D-B569-14AE213A2C18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>IA_1</t>
   </si>
@@ -68,85 +68,76 @@
     <t>identifier</t>
   </si>
   <si>
-    <t>a sus alumnos.</t>
-  </si>
-  <si>
-    <t>product_saltar_29</t>
-  </si>
-  <si>
-    <t>neutral</t>
-  </si>
-  <si>
     <t>critical</t>
   </si>
   <si>
-    <t>abarrotada.</t>
-  </si>
-  <si>
-    <t>unprod_echar_1</t>
-  </si>
-  <si>
-    <t>constraining</t>
-  </si>
-  <si>
-    <t>al final de la pelicula.</t>
-  </si>
-  <si>
-    <t>product_tirar_28</t>
-  </si>
-  <si>
-    <t>con sus amigos.</t>
-  </si>
-  <si>
-    <t>unprod_romper_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La maestra </t>
-  </si>
-  <si>
-    <t xml:space="preserve">La mujer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">La chica </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Francisco </t>
-  </si>
-  <si>
-    <t xml:space="preserve">salto a </t>
-  </si>
-  <si>
-    <t xml:space="preserve">se echo a </t>
-  </si>
-  <si>
-    <t xml:space="preserve">se tiro a </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rompio a </t>
-  </si>
-  <si>
-    <t xml:space="preserve">explicar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">caminar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">llorar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">hablar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">el tema </t>
-  </si>
-  <si>
-    <t xml:space="preserve">por la calle </t>
-  </si>
-  <si>
-    <t xml:space="preserve">desconsoladamente </t>
-  </si>
-  <si>
-    <t xml:space="preserve">de politica </t>
+    <t>slowly.</t>
+  </si>
+  <si>
+    <t>infreq_1</t>
+  </si>
+  <si>
+    <t>infrequent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The </t>
+  </si>
+  <si>
+    <t>mostly empty.</t>
+  </si>
+  <si>
+    <t>infreq_2</t>
+  </si>
+  <si>
+    <t>the sparrows.</t>
+  </si>
+  <si>
+    <t>freq_3</t>
+  </si>
+  <si>
+    <t>frequent</t>
+  </si>
+  <si>
+    <t>for many miles.</t>
+  </si>
+  <si>
+    <t>freq_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shiny </t>
+  </si>
+  <si>
+    <t xml:space="preserve">large </t>
+  </si>
+  <si>
+    <t xml:space="preserve">noisy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sandy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gondola </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mosque </t>
+  </si>
+  <si>
+    <t xml:space="preserve">chicken </t>
+  </si>
+  <si>
+    <t xml:space="preserve">beach </t>
+  </si>
+  <si>
+    <t xml:space="preserve">moved </t>
+  </si>
+  <si>
+    <t xml:space="preserve">remained </t>
+  </si>
+  <si>
+    <t xml:space="preserve">chased </t>
+  </si>
+  <si>
+    <t xml:space="preserve">stretched </t>
   </si>
 </sst>
 </file>
@@ -199,6 +190,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -501,7 +496,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,80 +544,80 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
       <c r="J2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3">
         <v>2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
@@ -631,48 +626,48 @@
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J4">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
       <c r="H5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J5">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>